<commit_message>
Chekpoint 3 - Visual Improvement starts
</commit_message>
<xml_diff>
--- a/AppFolder/StockIn.xlsx
+++ b/AppFolder/StockIn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CHAKH IT Management Software\WindowsApp1\AppFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C256AD8-591F-4793-BEA6-ED04BBD826E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C7DEB4-0733-4E3C-A93A-85B0A6E71188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>Entry Date</t>
   </si>
@@ -62,6 +62,24 @@
   </si>
   <si>
     <t>Cash</t>
+  </si>
+  <si>
+    <t>Rangeen Pop</t>
+  </si>
+  <si>
+    <t>Outer</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Jalebi Jelly</t>
+  </si>
+  <si>
+    <t>sc</t>
   </si>
 </sst>
 </file>
@@ -430,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -506,6 +524,236 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.64778935185185182</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>500</v>
+      </c>
+      <c r="G3">
+        <v>456</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.6731018518518519</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>500</v>
+      </c>
+      <c r="G4">
+        <v>456</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.68487268518518518</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>500</v>
+      </c>
+      <c r="G5">
+        <v>75</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5">
+        <v>50</v>
+      </c>
+      <c r="K5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.76513888888888892</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>1000</v>
+      </c>
+      <c r="H6">
+        <v>456</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.76613425925925926</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>60</v>
+      </c>
+      <c r="G7">
+        <v>900</v>
+      </c>
+      <c r="H7">
+        <v>654</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.77379629629629632</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
+        <v>1250</v>
+      </c>
+      <c r="H8">
+        <v>46</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.77614583333333331</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <v>1250</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Onlu Finances and Dashboard tabs remainng to be configured
</commit_message>
<xml_diff>
--- a/AppFolder/StockIn.xlsx
+++ b/AppFolder/StockIn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CHAKH IT Management Software\WindowsApp1\AppFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D857FDF-A604-422C-8E63-0FB16BC7535D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126193F9-84ED-4BE6-B3AF-D29CA1756EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="24">
   <si>
     <t>Entry Date</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Rangeen Pop Big</t>
+  </si>
+  <si>
+    <t>Test007</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1075,6 +1078,38 @@
         <v>13</v>
       </c>
     </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>45879</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.83199074074074075</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20">
+        <v>1250</v>
+      </c>
+      <c r="H20">
+        <v>12546</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>